<commit_message>
update lab results.txt for web tools
</commit_message>
<xml_diff>
--- a/Modules/Web_tools_for_genomic_epidemiology/lab_results.xlsx
+++ b/Modules/Web_tools_for_genomic_epidemiology/lab_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdiazcaballero/Documents/cgps/teaching/asuncion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4375E302-DC2E-6345-9C2B-E57325206782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8725A2F-1B65-FC4C-9C24-351E7A952362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{BA64E9F3-D88C-9C49-A084-22DFE9F308AD}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,10 +510,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -521,10 +521,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -576,10 +576,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -598,10 +598,10 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update lab_results of web tools
</commit_message>
<xml_diff>
--- a/Modules/Web_tools_for_genomic_epidemiology/lab_results.xlsx
+++ b/Modules/Web_tools_for_genomic_epidemiology/lab_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdiazcaballero/Documents/cgps/teaching/asuncion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8725A2F-1B65-FC4C-9C24-351E7A952362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C29239-61E6-F84F-9C1C-78FCBA690987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{BA64E9F3-D88C-9C49-A084-22DFE9F308AD}"/>
   </bookViews>
@@ -59,9 +59,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>cholerae</t>
-  </si>
-  <si>
     <t>Serotype</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>123456789-13</t>
+  </si>
+  <si>
+    <t>V. cholerae</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,7 +480,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -507,7 +507,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -529,7 +529,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -573,10 +573,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -595,10 +595,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>5</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>

</xml_diff>